<commit_message>
all data version not adding much relative to pca
</commit_message>
<xml_diff>
--- a/Output/Classifier Evaluation/Model Performance Table.xlsx
+++ b/Output/Classifier Evaluation/Model Performance Table.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,22 +476,22 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>All Features PCA</t>
+          <t>All Data</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>C: 0.1, class_weight: None, l1_ratio: 0.5, multi_class: ovr, penalty: elasticnet, solver: saga</t>
+          <t>C: 0.1, class_weight: balanced, l1_ratio: 1.0, multi_class: ovr, penalty: elasticnet, solver: saga</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.9921705813759787</v>
+        <v>0.9841745793769782</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.9048806550097142</v>
+        <v>0.915708021093533</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.890530557421088</v>
+        <v>0.9106783075889859</v>
       </c>
     </row>
     <row r="3">
@@ -502,48 +502,48 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Individual Features PCA</t>
+          <t>All Features PCA</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>C: 0.01, class_weight: balanced, l1_ratio: 0.25, multi_class: ovr, penalty: elasticnet, solver: saga</t>
+          <t>C: 0.1, class_weight: None, l1_ratio: 0.5, multi_class: ovr, penalty: elasticnet, solver: saga</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.9580209895052474</v>
+        <v>0.9921705813759787</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.9158759367194005</v>
+        <v>0.9048806550097142</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.9093351242444594</v>
+        <v>0.890530557421088</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>Logistic Regression</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>All Features PCA</t>
+          <t>Individual Features PCA</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>C: 0.1, degree: 2, gamma: 0.1, kernel: poly</t>
+          <t>C: 0.01, class_weight: balanced, l1_ratio: 0.25, multi_class: ovr, penalty: elasticnet, solver: saga</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1</v>
+        <v>0.9580209895052474</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.5032482653344436</v>
+        <v>0.9158759367194005</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.5742108797850907</v>
+        <v>0.9093351242444594</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +554,7 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>Individual Features PCA</t>
+          <t>All Features PCA</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
@@ -566,36 +566,36 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.5797078823202886</v>
+        <v>0.5032482653344436</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.6312961719274681</v>
+        <v>0.5742108797850907</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>XGBoost</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>All Features PCA</t>
+          <t>Individual Features PCA</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>colsample_bytree: 1, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
+          <t>C: 0.1, degree: 2, gamma: 0.1, kernel: poly</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.8555727171801276</v>
+        <v>0.5797078823202886</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.8629952988582942</v>
+        <v>0.6312961719274681</v>
       </c>
     </row>
     <row r="7">
@@ -606,21 +606,47 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Individual Features PCA</t>
+          <t>All Features PCA</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>colsample_bytree: 0.8, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
+          <t>colsample_bytree: 1, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="n">
+        <v>0.8555727171801276</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.8629952988582942</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Individual Features PCA</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>colsample_bytree: 0.8, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="n">
         <v>0.888055925617541</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F8" s="2" t="n">
         <v>0.8811282740094023</v>
       </c>
     </row>

</xml_diff>

<commit_message>
efficiency - accuracy table
</commit_message>
<xml_diff>
--- a/Output/Classifier Evaluation/Model Performance Table.xlsx
+++ b/Output/Classifier Evaluation/Model Performance Table.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,7 +606,7 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>All Features PCA</t>
+          <t>All Features</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
@@ -618,10 +618,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.8555727171801276</v>
+        <v>0.9093798223702472</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.8629952988582942</v>
+        <v>0.9012760241773002</v>
       </c>
     </row>
     <row r="8">
@@ -632,21 +632,47 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Individual Features PCA</t>
+          <t>All Features PCA</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>colsample_bytree: 0.8, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
+          <t>colsample_bytree: 1, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="n">
+        <v>0.8555727171801276</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.8629952988582942</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Individual Features PCA</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>colsample_bytree: 0.8, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="n">
         <v>0.888055925617541</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F9" s="2" t="n">
         <v>0.8811282740094023</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vgg only svm run
</commit_message>
<xml_diff>
--- a/Output/Classifier Evaluation/Model Performance Table.xlsx
+++ b/Output/Classifier Evaluation/Model Performance Table.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -601,27 +601,27 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>XGBoost</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>All Features</t>
+          <t>VGG</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>colsample_bytree: 1, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
+          <t>C: 1, degree: 2, gamma: 0.001, kernel: rbf</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>1</v>
+        <v>0.9431950691321006</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.9093798223702472</v>
+        <v>0.8697316125451013</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.9012760241773002</v>
+        <v>0.8643384822028207</v>
       </c>
     </row>
     <row r="8">
@@ -632,7 +632,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>All Features PCA</t>
+          <t>All Features</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
@@ -644,10 +644,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.8555727171801276</v>
+        <v>0.9093798223702472</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.8629952988582942</v>
+        <v>0.9012760241773002</v>
       </c>
     </row>
     <row r="9">
@@ -658,48 +658,48 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>Individual Features PCA</t>
+          <t>All Features PCA</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>colsample_bytree: 0.8, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
+          <t>colsample_bytree: 1, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.888055925617541</v>
+        <v>0.8555727171801276</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.8811282740094023</v>
+        <v>0.8629952988582942</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>XGBoost</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>All Features</t>
+          <t>Individual Features PCA</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>bootstrap: False, max_depth: 30, max_features: sqrt, min_samples_leaf: 2, min_samples_split: 5, n_estimators: 1000</t>
+          <t>colsample_bytree: 0.8, learning_rate: 0.3, max_depth: 3, n_estimators: 200, subsample: 0.8</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.861068276436303</v>
+        <v>0.888055925617541</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.847548690396239</v>
+        <v>0.8811282740094023</v>
       </c>
     </row>
     <row r="11">
@@ -710,22 +710,22 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>All Features PCA</t>
+          <t>All Features</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>bootstrap: False, max_depth: 60, max_features: sqrt, min_samples_leaf: 2, min_samples_split: 5, n_estimators: 1000</t>
+          <t>bootstrap: False, max_depth: 30, max_features: sqrt, min_samples_leaf: 2, min_samples_split: 5, n_estimators: 1000</t>
         </is>
       </c>
       <c r="D11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.6959852900360811</v>
+        <v>0.861068276436303</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.7004701141705842</v>
+        <v>0.847548690396239</v>
       </c>
     </row>
     <row r="12">
@@ -736,21 +736,47 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>Individual Features PCA</t>
+          <t>All Features PCA</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>bootstrap: False, max_depth: 50, max_features: sqrt, min_samples_leaf: 2, min_samples_split: 5, n_estimators: 1000</t>
+          <t>bootstrap: False, max_depth: 60, max_features: sqrt, min_samples_leaf: 2, min_samples_split: 5, n_estimators: 1000</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="n">
+        <v>0.6959852900360811</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0.7004701141705842</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>Individual Features PCA</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>bootstrap: False, max_depth: 50, max_features: sqrt, min_samples_leaf: 2, min_samples_split: 5, n_estimators: 1000</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="n">
         <v>0.8077581182348045</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F13" s="2" t="n">
         <v>0.7904633982538617</v>
       </c>
     </row>

</xml_diff>

<commit_message>
top3 featuers not reducing overfit
</commit_message>
<xml_diff>
--- a/Output/Classifier Evaluation/Model Performance Table.xlsx
+++ b/Output/Classifier Evaluation/Model Performance Table.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -637,14 +637,14 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>C: 1, class_weight: None, degree: 2, gamma: 0.001, kernel: rbf</t>
+          <t>C: 10.0, class_weight: balanced, gamma: scale, kernel: rbf</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.9431950691321006</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.8697316125451013</v>
+        <v>0.8697293921731891</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0.8643384822028207</v>
@@ -736,7 +736,7 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>VGG</t>
+          <t>Top3 Features</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
@@ -748,36 +748,36 @@
         <v>1</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.8637334165972801</v>
+        <v>0.8597356369691923</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.8542646071188718</v>
+        <v>0.8488918737407656</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>XGBoost</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>All Features</t>
+          <t>VGG</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>bootstrap: False, max_depth: 80, max_features: sqrt, min_samples_leaf: 1, n_estimators: 1500</t>
+          <t>learning_rate: 0.5, max_depth: 3, min_child_weight: 1, n_estimators: 300</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.8615681376630585</v>
+        <v>0.8637334165972801</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0.8529214237743452</v>
+        <v>0.8542646071188718</v>
       </c>
     </row>
     <row r="14">
@@ -788,22 +788,22 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>All Features PCA</t>
+          <t>All Features</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>bootstrap: False, max_depth: 60, max_features: sqrt, min_samples_leaf: 1, n_estimators: 1500</t>
+          <t>bootstrap: False, max_depth: 80, max_features: sqrt, min_samples_leaf: 1, n_estimators: 1500</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0.6989836247571468</v>
+        <v>0.8615681376630585</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0.7011417058428475</v>
+        <v>0.8529214237743452</v>
       </c>
     </row>
     <row r="15">
@@ -814,22 +814,74 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
+          <t>All Features PCA</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>bootstrap: False, max_depth: 60, max_features: sqrt, min_samples_leaf: 1, n_estimators: 1500</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.6989836247571468</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0.7011417058428475</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
           <t>Individual Features PCA</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>bootstrap: False, max_depth: 40, max_features: sqrt, min_samples_leaf: 1, n_estimators: 500</t>
         </is>
       </c>
-      <c r="D15" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="n">
+      <c r="D16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="n">
         <v>0.8084256175409381</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F16" s="2" t="n">
         <v>0.7897918065815984</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>Top3 Features</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>bootstrap: False, max_depth: 80, max_features: sqrt, min_samples_leaf: 2, n_estimators: 500</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0.7932697751873439</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>0.7575554063129617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>